<commit_message>
This is for new changes in release part 5
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC07_SearchCategory.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC07_SearchCategory.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97076169-39ED-4ED3-9BF5-779550899EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TC07_SearchCategory" sheetId="1" r:id="rId1"/>
     <sheet name="Testdata" sheetId="12" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>TestCase</t>
   </si>
@@ -143,12 +137,15 @@
   </si>
   <si>
     <t>JSElement</t>
+  </si>
+  <si>
+    <t>WAIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -557,11 +554,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -618,55 +615,73 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -678,7 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -821,7 +836,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus" xr:uid="{7E0DE4E8-1ECA-4F64-BF8F-E7BDBB151457}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -829,21 +844,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1040,24 +1040,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1074,4 +1072,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>